<commit_message>
Fixed logos and final energy and color coding
</commit_message>
<xml_diff>
--- a/scripts/Tech_names_Goa.xlsx
+++ b/scripts/Tech_names_Goa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shank\OneDrive\Documents\Github\Goa\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghosh\OneDrive - The Celestial Earth\Documents\Goa\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CD0063-BD94-4120-8136-5A2689546BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCCD691-3423-44AE-8F92-4D6E00858AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">primary_e!$A$1:$D$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">sectoral_mix!$A$1:$F$109</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="323">
   <si>
     <t>PWRSOL001A</t>
   </si>
@@ -1005,10 +1005,13 @@
     <t>Sector_Color</t>
   </si>
   <si>
-    <t>New_and_Renewed_PPA</t>
-  </si>
-  <si>
     <t>Solar</t>
+  </si>
+  <si>
+    <t>PPA(New/Renewed)</t>
+  </si>
+  <si>
+    <t>Gas PP</t>
   </si>
 </sst>
 </file>
@@ -1439,25 +1442,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="19.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="2"/>
+    <col min="5" max="5" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="2"/>
+    <col min="7" max="7" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1475,7 +1478,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1526,7 +1529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -1543,7 +1546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>222</v>
       </c>
@@ -1558,7 +1561,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>165</v>
       </c>
@@ -1575,7 +1578,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1593,7 +1596,7 @@
         <v>PWRWND001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>33</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>PWRWNDRPO</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>168</v>
       </c>
@@ -1623,12 +1626,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>164</v>
       </c>
       <c r="B11" t="s">
-        <v>265</v>
+        <v>321</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>313</v>
@@ -1637,7 +1640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1651,7 +1654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>219</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>220</v>
       </c>
@@ -1673,7 +1676,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>221</v>
       </c>
@@ -1684,12 +1687,12 @@
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>111</v>
+        <v>322</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>305</v>
@@ -1698,12 +1701,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>111</v>
+        <v>322</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>305</v>
@@ -1712,7 +1715,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -1726,7 +1729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -1754,7 +1757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
@@ -1768,7 +1771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>218</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>266</v>
       </c>
@@ -1818,109 +1821,109 @@
         <v>309</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="4"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="4"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="4"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="4"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="4"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" s="4"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="4"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="4"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="4"/>
     </row>
   </sheetData>
@@ -1940,13 +1943,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1962,7 +1965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1970,7 +1973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1978,7 +1981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1986,7 +1989,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -1994,7 +1997,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -2002,7 +2005,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -2010,7 +2013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>168</v>
       </c>
@@ -2018,7 +2021,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2026,7 +2029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2034,7 +2037,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2042,7 +2045,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>164</v>
       </c>
@@ -2051,7 +2054,7 @@
       </c>
       <c r="D13" s="13"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -2067,7 +2070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -2075,7 +2078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2083,7 +2086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2091,7 +2094,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -2099,7 +2102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>266</v>
       </c>
@@ -2116,19 +2119,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.140625" style="7"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -2156,7 +2159,7 @@
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -2173,7 +2176,7 @@
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>243</v>
       </c>
@@ -2188,7 +2191,7 @@
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -2205,7 +2208,7 @@
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -2219,7 +2222,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2234,7 +2237,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2248,7 +2251,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2262,7 +2265,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2276,7 +2279,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2290,7 +2293,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
-    <row r="12" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>222</v>
       </c>
@@ -2304,7 +2307,7 @@
       <c r="L12" s="6"/>
       <c r="M12" s="12"/>
     </row>
-    <row r="13" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>165</v>
       </c>
@@ -2318,7 +2321,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2330,7 +2333,7 @@
       </c>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2341,18 +2344,18 @@
         <v>311</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>164</v>
       </c>
       <c r="B16" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -2364,7 +2367,7 @@
       </c>
       <c r="M17" s="12"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -2376,7 +2379,7 @@
       </c>
       <c r="M18" s="12"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -2388,7 +2391,7 @@
       </c>
       <c r="M19" s="12"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>213</v>
       </c>
@@ -2400,7 +2403,7 @@
       </c>
       <c r="M20" s="12"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>104</v>
       </c>
@@ -2412,7 +2415,7 @@
       </c>
       <c r="M21" s="12"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>215</v>
       </c>
@@ -2424,7 +2427,7 @@
       </c>
       <c r="M22" s="12"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>214</v>
       </c>
@@ -2436,7 +2439,7 @@
       </c>
       <c r="M23" s="12"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2451,7 +2454,7 @@
       </c>
       <c r="M24" s="12"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>101</v>
       </c>
@@ -2466,7 +2469,7 @@
       </c>
       <c r="M25" s="12"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>171</v>
       </c>
@@ -2481,7 +2484,7 @@
       </c>
       <c r="M26" s="12"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>216</v>
       </c>
@@ -2496,7 +2499,7 @@
       </c>
       <c r="M27" s="12"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>266</v>
       </c>
@@ -2507,16 +2510,16 @@
         <v>309</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M29" s="12"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M30" s="12"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="M31" s="12"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K32" s="14"/>
       <c r="M32" s="12"/>
     </row>
@@ -2538,17 +2541,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -2562,7 +2565,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>134</v>
       </c>
@@ -2575,7 +2578,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>246</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>135</v>
       </c>
@@ -2600,7 +2603,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>136</v>
       </c>
@@ -2613,7 +2616,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>52</v>
       </c>
@@ -2626,7 +2629,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>245</v>
       </c>
@@ -2638,7 +2641,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>117</v>
       </c>
@@ -2651,7 +2654,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>116</v>
       </c>
@@ -2664,7 +2667,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>118</v>
       </c>
@@ -2677,7 +2680,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>119</v>
       </c>
@@ -2690,7 +2693,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>137</v>
       </c>
@@ -2703,7 +2706,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>138</v>
       </c>
@@ -2716,7 +2719,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>139</v>
       </c>
@@ -2729,7 +2732,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -2742,7 +2745,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>244</v>
       </c>
@@ -2754,7 +2757,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>55</v>
       </c>
@@ -2767,7 +2770,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>128</v>
       </c>
@@ -2780,7 +2783,7 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>120</v>
       </c>
@@ -2793,7 +2796,7 @@
       </c>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2806,7 +2809,7 @@
       </c>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>124</v>
       </c>
@@ -2819,7 +2822,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>131</v>
       </c>
@@ -2832,7 +2835,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>123</v>
       </c>
@@ -2845,7 +2848,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>132</v>
       </c>
@@ -2858,7 +2861,7 @@
       </c>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>127</v>
       </c>
@@ -2871,7 +2874,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>129</v>
       </c>
@@ -2884,7 +2887,7 @@
       </c>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>121</v>
       </c>
@@ -2897,7 +2900,7 @@
       </c>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -2910,7 +2913,7 @@
       </c>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>125</v>
       </c>
@@ -2923,7 +2926,7 @@
       </c>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>133</v>
       </c>
@@ -2936,7 +2939,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>130</v>
       </c>
@@ -2949,7 +2952,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>122</v>
       </c>
@@ -2962,7 +2965,7 @@
       </c>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>58</v>
       </c>
@@ -2975,7 +2978,7 @@
       </c>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>126</v>
       </c>
@@ -2988,7 +2991,7 @@
       </c>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>41</v>
       </c>
@@ -3001,7 +3004,7 @@
       </c>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>49</v>
       </c>
@@ -3014,7 +3017,7 @@
       </c>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>38</v>
       </c>
@@ -3027,7 +3030,7 @@
       </c>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>46</v>
       </c>
@@ -3040,7 +3043,7 @@
       </c>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>42</v>
       </c>
@@ -3053,7 +3056,7 @@
       </c>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>50</v>
       </c>
@@ -3066,7 +3069,7 @@
       </c>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>39</v>
       </c>
@@ -3079,7 +3082,7 @@
       </c>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>47</v>
       </c>
@@ -3092,7 +3095,7 @@
       </c>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>115</v>
       </c>
@@ -3105,7 +3108,7 @@
       </c>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>36</v>
       </c>
@@ -3118,7 +3121,7 @@
       </c>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>44</v>
       </c>
@@ -3131,7 +3134,7 @@
       </c>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>112</v>
       </c>
@@ -3144,7 +3147,7 @@
       </c>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>113</v>
       </c>
@@ -3157,7 +3160,7 @@
       </c>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>114</v>
       </c>
@@ -3170,7 +3173,7 @@
       </c>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>40</v>
       </c>
@@ -3183,7 +3186,7 @@
       </c>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>48</v>
       </c>
@@ -3196,7 +3199,7 @@
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>35</v>
       </c>
@@ -3209,7 +3212,7 @@
       </c>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>43</v>
       </c>
@@ -3222,7 +3225,7 @@
       </c>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>37</v>
       </c>
@@ -3235,7 +3238,7 @@
       </c>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>45</v>
       </c>
@@ -3248,7 +3251,7 @@
       </c>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>140</v>
       </c>
@@ -3261,7 +3264,7 @@
       </c>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>171</v>
       </c>
@@ -3274,7 +3277,7 @@
       </c>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>145</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>144</v>
       </c>
@@ -3299,7 +3302,7 @@
       </c>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>142</v>
       </c>
@@ -3312,7 +3315,7 @@
       </c>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>141</v>
       </c>
@@ -3325,7 +3328,7 @@
       </c>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>143</v>
       </c>
@@ -3338,7 +3341,7 @@
       </c>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>147</v>
       </c>
@@ -3351,7 +3354,7 @@
       </c>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>146</v>
       </c>
@@ -3364,7 +3367,7 @@
       </c>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>149</v>
       </c>
@@ -3377,7 +3380,7 @@
       </c>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>148</v>
       </c>
@@ -3409,17 +3412,17 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="7"/>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="7"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -3438,7 +3441,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>+final_e!A17</f>
         <v>DEMINDBIOOTH</v>
@@ -3447,7 +3450,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>+final_e!A35</f>
         <v>DEMRESBGSCKG</v>
@@ -3456,7 +3459,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>+final_e!A36</f>
         <v>DEMRESBGSCKGr</v>
@@ -3465,7 +3468,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>+final_e!A37</f>
         <v>DEMRESBIICKG</v>
@@ -3474,7 +3477,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>+final_e!A38</f>
         <v>DEMRESBIICKGr</v>
@@ -3483,7 +3486,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>+final_e!A39</f>
         <v>DEMRESBIOCKG</v>
@@ -3492,7 +3495,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>+final_e!A40</f>
         <v>DEMRESBIOCKGr</v>
@@ -3501,7 +3504,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>+final_e!A56</f>
         <v>MINATF</v>
@@ -3510,7 +3513,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>+final_e!A57</f>
         <v>TRANBIODSL</v>
@@ -3519,7 +3522,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>+final_e!A18</f>
         <v>DEMINDCOAMSH</v>
@@ -3528,7 +3531,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>+final_e!A19</f>
         <v>DEMINDCOAMSM</v>
@@ -3537,7 +3540,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>+final_e!A20</f>
         <v>DEMINDCOAOTH</v>
@@ -3546,7 +3549,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f>+final_e!A21</f>
         <v>DEMINDCOASTL</v>
@@ -3555,7 +3558,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f>+final_e!A41</f>
         <v>DEMRESCOACKG</v>
@@ -3564,7 +3567,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>+final_e!A42</f>
         <v>DEMRESCOACKGr</v>
@@ -3573,7 +3576,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f>+final_e!A3</f>
         <v>DEMAGRCSTBDSL</v>
@@ -3582,7 +3585,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>+final_e!A4</f>
         <v>DEMAGRFPR</v>
@@ -3591,7 +3594,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f>+final_e!A8</f>
         <v>DEMCOMAPP</v>
@@ -3600,7 +3603,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f>+final_e!A9</f>
         <v>DEMCOMHAC</v>
@@ -3609,7 +3612,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>+final_e!A11</f>
         <v>DEMCOMOTH</v>
@@ -3618,7 +3621,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>+final_e!A12</f>
         <v>DEMFSHCST</v>
@@ -3627,7 +3630,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f>+final_e!A13</f>
         <v>DEMFSHFPR</v>
@@ -3636,7 +3639,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>+final_e!A14</f>
         <v>DEMFSHPUM</v>
@@ -3645,7 +3648,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>+final_e!A22</f>
         <v>DEMINDELECMSH</v>
@@ -3654,7 +3657,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f>+final_e!A23</f>
         <v>DEMINDELECMSM</v>
@@ -3663,7 +3666,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f>+final_e!A24</f>
         <v>DEMINDELECOTH</v>
@@ -3672,7 +3675,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f>+final_e!A25</f>
         <v>DEMINDELECSTL</v>
@@ -3681,7 +3684,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f>+final_e!A43</f>
         <v>DEMRESELCAPP</v>
@@ -3690,7 +3693,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f>+final_e!A44</f>
         <v>DEMRESELCCKG</v>
@@ -3699,7 +3702,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f>+final_e!A45</f>
         <v>DEMRESELCCKGr</v>
@@ -3708,7 +3711,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f>+final_e!A46</f>
         <v>DEMRESELCHAC</v>
@@ -3717,7 +3720,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f>+final_e!A47</f>
         <v>DEMRESELCHWT</v>
@@ -3726,7 +3729,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f>+final_e!A48</f>
         <v>DEMRESELCLGT</v>
@@ -3735,7 +3738,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f>+final_e!A60</f>
         <v>TRANDSL</v>
@@ -3744,7 +3747,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f>+final_e!A26</f>
         <v>DEMINDGASMSH</v>
@@ -3753,7 +3756,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f>+final_e!A27</f>
         <v>DEMINDGASMSM</v>
@@ -3762,7 +3765,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f>+final_e!A28</f>
         <v>DEMINDGASOTH</v>
@@ -3771,7 +3774,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f>+final_e!A29</f>
         <v>DEMINDGASSTL</v>
@@ -3780,7 +3783,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f>+final_e!A51</f>
         <v>DEMRESLPGCKG</v>
@@ -3789,7 +3792,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f>+final_e!A52</f>
         <v>DEMRESLPGCKGr</v>
@@ -3798,7 +3801,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f>+final_e!A53</f>
         <v>DEMRESPNGCKG</v>
@@ -3807,7 +3810,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f>+final_e!A54</f>
         <v>DEMRESPNGCKGr</v>
@@ -3816,7 +3819,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f>+final_e!A58</f>
         <v>TRANBIOETH</v>
@@ -3825,7 +3828,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f>+final_e!A62</f>
         <v>TRANH2</v>
@@ -3834,7 +3837,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f>+final_e!A63</f>
         <v>TRANLNG</v>
@@ -3843,7 +3846,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f>+final_e!A30</f>
         <v>DEMINDH2OTH</v>
@@ -3852,7 +3855,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f>+final_e!A61</f>
         <v>TRANELEC</v>
@@ -3861,7 +3864,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f>+final_e!A2</f>
         <v>DEMAGRCST</v>
@@ -3870,7 +3873,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f>+final_e!A5</f>
         <v>DEMAGRPUM</v>
@@ -3880,7 +3883,7 @@
       </c>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f>+final_e!A15</f>
         <v>DEMFSHVES</v>
@@ -3889,7 +3892,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f>+final_e!A31</f>
         <v>DEMINDOILMSH</v>
@@ -3898,7 +3901,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>+final_e!A32</f>
         <v>DEMINDOILMSM</v>
@@ -3907,7 +3910,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f>+final_e!A33</f>
         <v>DEMINDOILOTH</v>
@@ -3916,7 +3919,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f>+final_e!A34</f>
         <v>DEMINDOILSTL</v>
@@ -3925,7 +3928,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f>+final_e!A49</f>
         <v>DEMRESKERCKG</v>
@@ -3934,7 +3937,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f>+final_e!A50</f>
         <v>DEMRESKERCKGr</v>
@@ -3943,7 +3946,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f>+final_e!A59</f>
         <v>TRANCNG</v>
@@ -3952,7 +3955,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f>+final_e!A64</f>
         <v>TRANLPG</v>
@@ -3961,7 +3964,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>171</v>
       </c>
@@ -3969,7 +3972,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f>+final_e!A10</f>
         <v>DEMCOMHWT</v>
@@ -3978,7 +3981,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f>+final_e!A55</f>
         <v>DEMRESSOLHWT</v>
@@ -4000,20 +4003,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="20.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>30</v>
       </c>
@@ -4033,7 +4036,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>134</v>
       </c>
@@ -4054,7 +4057,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>246</v>
       </c>
@@ -4074,7 +4077,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>135</v>
       </c>
@@ -4095,7 +4098,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>136</v>
       </c>
@@ -4103,7 +4106,7 @@
         <v>211</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D5" s="7" t="str">
         <f>+CONCATENATE(B5,"-",C5)</f>
@@ -4116,7 +4119,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>52</v>
       </c>
@@ -4137,7 +4140,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>245</v>
       </c>
@@ -4157,7 +4160,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>117</v>
       </c>
@@ -4178,7 +4181,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>116</v>
       </c>
@@ -4199,7 +4202,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>118</v>
       </c>
@@ -4220,7 +4223,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>119</v>
       </c>
@@ -4241,7 +4244,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>137</v>
       </c>
@@ -4262,7 +4265,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>138</v>
       </c>
@@ -4283,7 +4286,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>139</v>
       </c>
@@ -4304,7 +4307,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4325,7 +4328,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>244</v>
       </c>
@@ -4345,7 +4348,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>55</v>
       </c>
@@ -4366,7 +4369,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>128</v>
       </c>
@@ -4387,7 +4390,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>120</v>
       </c>
@@ -4408,7 +4411,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -4429,7 +4432,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>124</v>
       </c>
@@ -4450,7 +4453,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>131</v>
       </c>
@@ -4471,7 +4474,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>123</v>
       </c>
@@ -4492,7 +4495,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>132</v>
       </c>
@@ -4513,7 +4516,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>127</v>
       </c>
@@ -4534,7 +4537,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>129</v>
       </c>
@@ -4555,7 +4558,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>121</v>
       </c>
@@ -4576,7 +4579,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>57</v>
       </c>
@@ -4597,7 +4600,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>125</v>
       </c>
@@ -4618,7 +4621,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>133</v>
       </c>
@@ -4639,7 +4642,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>130</v>
       </c>
@@ -4660,7 +4663,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>58</v>
       </c>
@@ -4681,7 +4684,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>41</v>
       </c>
@@ -4702,7 +4705,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>49</v>
       </c>
@@ -4723,7 +4726,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>38</v>
       </c>
@@ -4744,7 +4747,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>46</v>
       </c>
@@ -4765,7 +4768,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>42</v>
       </c>
@@ -4786,7 +4789,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>50</v>
       </c>
@@ -4807,7 +4810,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>39</v>
       </c>
@@ -4828,7 +4831,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -4849,7 +4852,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>115</v>
       </c>
@@ -4870,7 +4873,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>36</v>
       </c>
@@ -4891,7 +4894,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>44</v>
       </c>
@@ -4912,7 +4915,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>112</v>
       </c>
@@ -4933,7 +4936,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>113</v>
       </c>
@@ -4954,7 +4957,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>114</v>
       </c>
@@ -4975,7 +4978,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>40</v>
       </c>
@@ -4995,7 +4998,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>48</v>
       </c>
@@ -5015,7 +5018,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>35</v>
       </c>
@@ -5036,7 +5039,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>43</v>
       </c>
@@ -5057,7 +5060,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>37</v>
       </c>
@@ -5078,7 +5081,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>45</v>
       </c>
@@ -5099,7 +5102,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>140</v>
       </c>
@@ -5120,7 +5123,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>95</v>
       </c>
@@ -5140,7 +5143,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>96</v>
       </c>
@@ -5160,7 +5163,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>94</v>
       </c>
@@ -5180,7 +5183,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>93</v>
       </c>
@@ -5200,7 +5203,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>252</v>
       </c>
@@ -5220,7 +5223,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>87</v>
       </c>
@@ -5240,7 +5243,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>88</v>
       </c>
@@ -5260,7 +5263,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>86</v>
       </c>
@@ -5280,7 +5283,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>85</v>
       </c>
@@ -5300,7 +5303,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>226</v>
       </c>
@@ -5320,7 +5323,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>253</v>
       </c>
@@ -5340,7 +5343,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>91</v>
       </c>
@@ -5360,7 +5363,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>92</v>
       </c>
@@ -5380,7 +5383,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>90</v>
       </c>
@@ -5400,7 +5403,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>89</v>
       </c>
@@ -5420,7 +5423,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>227</v>
       </c>
@@ -5440,7 +5443,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
         <v>71</v>
       </c>
@@ -5460,7 +5463,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>70</v>
       </c>
@@ -5480,7 +5483,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>233</v>
       </c>
@@ -5500,7 +5503,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="7" t="s">
         <v>232</v>
       </c>
@@ -5520,7 +5523,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
         <v>250</v>
       </c>
@@ -5540,7 +5543,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>72</v>
       </c>
@@ -5560,7 +5563,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="7" t="s">
         <v>76</v>
       </c>
@@ -5580,7 +5583,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
         <v>73</v>
       </c>
@@ -5600,7 +5603,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="7" t="s">
         <v>75</v>
       </c>
@@ -5620,7 +5623,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="7" t="s">
         <v>74</v>
       </c>
@@ -5640,7 +5643,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="7" t="s">
         <v>83</v>
       </c>
@@ -5660,7 +5663,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>257</v>
       </c>
@@ -5680,7 +5683,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
         <v>63</v>
       </c>
@@ -5700,7 +5703,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
         <v>64</v>
       </c>
@@ -5720,7 +5723,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="7" t="s">
         <v>65</v>
       </c>
@@ -5740,7 +5743,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="7" t="s">
         <v>62</v>
       </c>
@@ -5760,7 +5763,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="7" t="s">
         <v>172</v>
       </c>
@@ -5780,7 +5783,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="7" t="s">
         <v>176</v>
       </c>
@@ -5800,7 +5803,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="7" t="s">
         <v>177</v>
       </c>
@@ -5820,7 +5823,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
         <v>61</v>
       </c>
@@ -5840,7 +5843,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="7" t="s">
         <v>68</v>
       </c>
@@ -5860,7 +5863,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
         <v>69</v>
       </c>
@@ -5880,7 +5883,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="7" t="s">
         <v>60</v>
       </c>
@@ -5900,7 +5903,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="7" t="s">
         <v>59</v>
       </c>
@@ -5920,7 +5923,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="7" t="s">
         <v>251</v>
       </c>
@@ -5940,7 +5943,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>84</v>
       </c>
@@ -5960,7 +5963,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>249</v>
       </c>
@@ -5980,7 +5983,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="7" t="s">
         <v>67</v>
       </c>
@@ -6000,7 +6003,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
         <v>66</v>
       </c>
@@ -6020,7 +6023,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="7" t="s">
         <v>174</v>
       </c>
@@ -6040,7 +6043,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="7" t="s">
         <v>175</v>
       </c>
@@ -6060,7 +6063,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="7" t="s">
         <v>173</v>
       </c>
@@ -6080,7 +6083,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="7" t="s">
         <v>82</v>
       </c>
@@ -6100,7 +6103,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="7" t="s">
         <v>81</v>
       </c>
@@ -6120,7 +6123,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="7" t="s">
         <v>254</v>
       </c>
@@ -6140,7 +6143,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="7" t="s">
         <v>77</v>
       </c>
@@ -6160,7 +6163,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="7" t="s">
         <v>80</v>
       </c>
@@ -6180,7 +6183,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="7" t="s">
         <v>78</v>
       </c>
@@ -6200,7 +6203,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="7" t="s">
         <v>79</v>
       </c>
@@ -6220,7 +6223,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="7" t="s">
         <v>178</v>
       </c>

</xml_diff>